<commit_message>
adding overall dash, renaming/organizing files for logical structure
</commit_message>
<xml_diff>
--- a/within_states/within_state_disparity_data/community_living_within_2022_excel.xlsx
+++ b/within_states/within_state_disparity_data/community_living_within_2022_excel.xlsx
@@ -37,7 +37,7 @@
     <t>z_disparity_nursing_18_64_pct</t>
   </si>
   <si>
-    <t>index_disparity_nursing_18_64_pct</t>
+    <t>EQ_index_disparity_nursing_18_64_pct</t>
   </si>
   <si>
     <t>pwd_grpquarters_institution_pct</t>
@@ -52,7 +52,7 @@
     <t>z_disparity_grpquarters_institution_pct</t>
   </si>
   <si>
-    <t>index_disparity_grpquarters_institution_pct</t>
+    <t>EQ_index_disparity_grpquarters_institution_pct</t>
   </si>
   <si>
     <t>pwd_grpquarters_noninstitution_pct</t>
@@ -67,7 +67,7 @@
     <t>z_disparity_grpquarters_noninstitution_pct</t>
   </si>
   <si>
-    <t>index_disparity_grpquarters_noninstitution_pct</t>
+    <t>EQ_index_disparity_grpquarters_noninstitution_pct</t>
   </si>
   <si>
     <t>pwd_home_pct</t>
@@ -82,7 +82,7 @@
     <t>z_disparity_home_pct</t>
   </si>
   <si>
-    <t>index_disparity_home_pct</t>
+    <t>EQ_index_disparity_home_pct</t>
   </si>
   <si>
     <t>pwd_corrections_pct</t>
@@ -97,7 +97,7 @@
     <t>z_disparity_corrections_pct</t>
   </si>
   <si>
-    <t>index_disparity_corrections_pct</t>
+    <t>EQ_index_disparity_corrections_pct</t>
   </si>
   <si>
     <t>Community Living Equity Index</t>

</xml_diff>